<commit_message>
112-Music Player Global State Tracking
</commit_message>
<xml_diff>
--- a/dokumenti/Ucesce_clanova_u_implementaciji_v1.xlsx
+++ b/dokumenti/Ucesce_clanova_u_implementaciji_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Preuzimanja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\808Music\dokumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17843DBA-0228-4F80-9C52-B8D600D7D0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD18028C-4829-4ECF-B843-246899914A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="16740" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>Učešće članova u implementaciji po funkcionalnostima</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Plan</t>
-  </si>
-  <si>
-    <t>Stanje na dan 1.1.2019</t>
   </si>
   <si>
     <t>procentualno učešće</t>
@@ -63,25 +60,10 @@
     <t>U koje tabele se dodaju (ili mijenjaju) zapisi za navedenu funkcionalnost</t>
   </si>
   <si>
-    <t>Član 1</t>
-  </si>
-  <si>
-    <t>Član 2</t>
-  </si>
-  <si>
     <t>Član 3</t>
   </si>
   <si>
     <t>Sumarno treba biti 100%</t>
-  </si>
-  <si>
-    <t>Administrator</t>
-  </si>
-  <si>
-    <t>Tabela23</t>
-  </si>
-  <si>
-    <t>Tabela24</t>
   </si>
   <si>
     <t>Ukupni bodovi:</t>
@@ -111,12 +93,6 @@
     <t>Ukupno</t>
   </si>
   <si>
-    <t>Tabela21</t>
-  </si>
-  <si>
-    <t>Tabela22</t>
-  </si>
-  <si>
     <t>Marko</t>
   </si>
   <si>
@@ -141,43 +117,15 @@
     <t>View analytics</t>
   </si>
   <si>
-    <t>Manage profile</t>
-  </si>
-  <si>
     <t>Music streaming</t>
   </si>
   <si>
     <t>Manage playlists</t>
   </si>
   <si>
-    <t>Follow artists</t>
-  </si>
-  <si>
-    <t>Buy products</t>
-  </si>
-  <si>
     <t>Manage subscriptions</t>
   </si>
   <si>
-    <t>Download owned content</t>
-  </si>
-  <si>
-    <t>Share music in app</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overview of reports
-</t>
-  </si>
-  <si>
-    <t>Ban users</t>
-  </si>
-  <si>
-    <t>Delete tracks &amp; content</t>
-  </si>
-  <si>
-    <t>Manage content based on reports</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
@@ -187,9 +135,6 @@
     <t>View notifications</t>
   </si>
   <si>
-    <t>Report music</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -220,18 +165,12 @@
     <t>TrackPlaylist</t>
   </si>
   <si>
-    <t>Library</t>
-  </si>
-  <si>
     <t>Subscriptions</t>
   </si>
   <si>
     <t>Follows</t>
   </si>
   <si>
-    <t>UserArtistRoles</t>
-  </si>
-  <si>
     <t>Order</t>
   </si>
   <si>
@@ -244,22 +183,103 @@
     <t>ProductPhoto</t>
   </si>
   <si>
-    <t>LibraryProducts</t>
-  </si>
-  <si>
     <t>Orders, OrderDetails</t>
   </si>
   <si>
-    <t>Track, ArtistTrack, Album</t>
-  </si>
-  <si>
-    <t>Orders, OrderDetails, LibraryProducts</t>
-  </si>
-  <si>
     <t>Playlist, TrackPlaylist</t>
   </si>
   <si>
-    <t>Product, ProductPhoto</t>
+    <t>Stanje na dan 3.2.2025.</t>
+  </si>
+  <si>
+    <t>TrackStream</t>
+  </si>
+  <si>
+    <t>Track, ArtistTrack, Album, Notification</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Product, ProductPhoto, Notification</t>
+  </si>
+  <si>
+    <t>Notification, ReadNotification, MyAppUserPreferences</t>
+  </si>
+  <si>
+    <t>ReadNotification</t>
+  </si>
+  <si>
+    <t>MyAppUserPreferences</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Share music in app/social media</t>
+  </si>
+  <si>
+    <t>UserChat, ChatMessage</t>
+  </si>
+  <si>
+    <t>ChatMessage</t>
+  </si>
+  <si>
+    <t>UserChat</t>
+  </si>
+  <si>
+    <t>Manage profiles</t>
+  </si>
+  <si>
+    <t>UserArtistRole</t>
+  </si>
+  <si>
+    <t>MyUserArtistInvite</t>
+  </si>
+  <si>
+    <t>Artist, MyAppUser, UserArtist, UserArtistRole, MyUserArtistInvite</t>
+  </si>
+  <si>
+    <t>View profiles</t>
+  </si>
+  <si>
+    <t>(reads from) Product, Follows, TrackStream</t>
+  </si>
+  <si>
+    <t>(reads from) Orders, OrderDetails</t>
+  </si>
+  <si>
+    <t>Follow artists &amp; Users</t>
+  </si>
+  <si>
+    <t>Follows, FollowsForUser</t>
+  </si>
+  <si>
+    <t>(reads from) Track, Artist, MyAppUser, Product, Event</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>(reads from) Track, Artist, MyAppUser, Album</t>
+  </si>
+  <si>
+    <t>Search, Filter, Sort Products in Shop</t>
+  </si>
+  <si>
+    <t>(reads from) Product</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>(reads from) Track</t>
+  </si>
+  <si>
+    <t>Buy &amp; view products</t>
   </si>
 </sst>
 </file>
@@ -529,7 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,27 +640,30 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -659,8 +682,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1102,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,16 +1143,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I5" s="9"/>
@@ -1148,106 +1171,106 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="25"/>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="37"/>
+      <c r="J7" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="36"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="33"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="25"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="37"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="36"/>
     </row>
     <row r="9" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="21" t="s">
+      <c r="E9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>10</v>
-      </c>
       <c r="H9" s="23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I9" s="12"/>
       <c r="J9" s="18" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M9" s="19"/>
       <c r="N9" s="20"/>
       <c r="O9" s="18" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q9" s="18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
-        <v>27</v>
+      <c r="A10" s="40" t="s">
+        <v>19</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C10" s="10">
         <v>3</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -1264,7 +1287,7 @@
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="4">
         <v>0</v>
@@ -1274,12 +1297,12 @@
       </c>
       <c r="M10" s="8">
         <f>SUM(J10:L10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="14"/>
       <c r="O10" s="15">
         <f>$C10*J10</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P10" s="15">
         <f t="shared" ref="P10:Q10" si="0">$C10*K10</f>
@@ -1291,15 +1314,15 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C11" s="10">
         <v>3</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -1311,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" ref="H11:H36" si="1">SUM(E11:G11)</f>
+        <f t="shared" ref="H11:H27" si="1">SUM(E11:G11)</f>
         <v>1</v>
       </c>
       <c r="I11" s="13"/>
@@ -1319,33 +1342,33 @@
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="4">
         <v>0</v>
       </c>
       <c r="M11" s="8">
-        <f t="shared" ref="M11:M36" si="2">SUM(J11:L11)</f>
-        <v>0</v>
+        <f t="shared" ref="M11:M35" si="2">SUM(J11:L11)</f>
+        <v>1</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="15">
-        <f t="shared" ref="O11:O28" si="3">$C11*J11</f>
+        <f t="shared" ref="O11:O27" si="3">$C11*J11</f>
         <v>0</v>
       </c>
       <c r="P11" s="15">
-        <f t="shared" ref="P11:P28" si="4">$C11*K11</f>
-        <v>0</v>
+        <f t="shared" ref="P11:P27" si="4">$C11*K11</f>
+        <v>3</v>
       </c>
       <c r="Q11" s="15">
-        <f t="shared" ref="Q11:Q28" si="5">$C11*L11</f>
+        <f t="shared" ref="Q11:Q27" si="5">$C11*L11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C12" s="10">
         <v>2</v>
@@ -1371,14 +1394,14 @@
         <v>0</v>
       </c>
       <c r="K12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="4">
         <v>0</v>
       </c>
       <c r="M12" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="14"/>
       <c r="O12" s="15">
@@ -1387,7 +1410,7 @@
       </c>
       <c r="P12" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="15">
         <f t="shared" si="5"/>
@@ -1395,14 +1418,16 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C13" s="10">
-        <v>4</v>
-      </c>
-      <c r="D13" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
@@ -1421,14 +1446,14 @@
         <v>0</v>
       </c>
       <c r="K13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="4">
         <v>0</v>
       </c>
       <c r="M13" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="15">
@@ -1437,7 +1462,7 @@
       </c>
       <c r="P13" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q13" s="15">
         <f t="shared" si="5"/>
@@ -1445,21 +1470,23 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="40" t="s">
+        <v>20</v>
+      </c>
       <c r="B14" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C14" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -1470,7 +1497,7 @@
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="4">
         <v>0</v>
@@ -1480,34 +1507,32 @@
       </c>
       <c r="M14" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="14"/>
       <c r="O14" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="O14" si="6">$C14*J14</f>
+        <v>5</v>
       </c>
       <c r="P14" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="P14" si="7">$C14*K14</f>
         <v>0</v>
       </c>
       <c r="Q14" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="Q14" si="8">$C14*L14</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
-        <v>28</v>
-      </c>
+      <c r="A15" s="41"/>
       <c r="B15" s="6" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C15" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
@@ -1524,7 +1549,7 @@
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="4">
         <v>0</v>
@@ -1534,36 +1559,38 @@
       </c>
       <c r="M15" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="14"/>
       <c r="O15" s="15">
-        <f t="shared" ref="O15" si="6">$C15*J15</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
       <c r="P15" s="15">
-        <f t="shared" ref="P15" si="7">$C15*K15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q15" s="15">
-        <f t="shared" ref="Q15" si="8">$C15*L15</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C16" s="10">
         <v>3</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="E16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="4">
         <v>0</v>
@@ -1577,14 +1604,14 @@
         <v>0</v>
       </c>
       <c r="K16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="4">
         <v>0</v>
       </c>
       <c r="M16" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="14"/>
       <c r="O16" s="15">
@@ -1593,7 +1620,7 @@
       </c>
       <c r="P16" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q16" s="15">
         <f t="shared" si="5"/>
@@ -1601,21 +1628,21 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="6" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="C17" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F17" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -1626,26 +1653,26 @@
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K17" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L17" s="4">
         <v>0</v>
       </c>
       <c r="M17" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="14"/>
       <c r="O17" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="P17" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Q17" s="15">
         <f t="shared" si="5"/>
@@ -1653,23 +1680,23 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="6" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="C18" s="10">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
         <v>0</v>
       </c>
       <c r="H18" s="8">
@@ -1681,14 +1708,14 @@
         <v>0</v>
       </c>
       <c r="K18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="4">
         <v>0</v>
       </c>
       <c r="M18" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="14"/>
       <c r="O18" s="15">
@@ -1697,7 +1724,7 @@
       </c>
       <c r="P18" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q18" s="15">
         <f t="shared" si="5"/>
@@ -1705,15 +1732,15 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C19" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="E19" s="4">
         <v>0</v>
@@ -1733,14 +1760,14 @@
         <v>0</v>
       </c>
       <c r="K19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="4">
         <v>0</v>
       </c>
       <c r="M19" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="14"/>
       <c r="O19" s="15">
@@ -1749,7 +1776,7 @@
       </c>
       <c r="P19" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q19" s="15">
         <f t="shared" si="5"/>
@@ -1757,21 +1784,21 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C20" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
@@ -1782,7 +1809,7 @@
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="4">
         <v>0</v>
@@ -1792,31 +1819,33 @@
       </c>
       <c r="M20" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="14"/>
       <c r="O20" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="O20:O21" si="9">$C20*J20</f>
+        <v>5</v>
       </c>
       <c r="P20" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="P20:P21" si="10">$C20*K20</f>
         <v>0</v>
       </c>
       <c r="Q20" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="Q20:Q21" si="11">$C20*L20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="10">
-        <v>2</v>
-      </c>
-      <c r="D21" s="6"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="26">
+        <v>8</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="E21" s="4">
         <v>1</v>
       </c>
@@ -1832,7 +1861,7 @@
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="4">
         <v>0</v>
@@ -1842,42 +1871,44 @@
       </c>
       <c r="M21" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="14"/>
       <c r="O21" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>8</v>
       </c>
       <c r="P21" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q21" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="10">
-        <v>4</v>
-      </c>
-      <c r="D22" s="6"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="26">
+        <v>5</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="E22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H22" si="12">SUM(E22:G22)</f>
         <v>1</v>
       </c>
       <c r="I22" s="13"/>
@@ -1885,45 +1916,47 @@
         <v>0</v>
       </c>
       <c r="K22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="4">
         <v>0</v>
       </c>
       <c r="M22" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="M22" si="13">SUM(J22:L22)</f>
+        <v>1</v>
       </c>
       <c r="N22" s="14"/>
       <c r="O22" s="15">
-        <f t="shared" ref="O22:O23" si="9">$C22*J22</f>
+        <f t="shared" ref="O22" si="14">$C22*J22</f>
         <v>0</v>
       </c>
       <c r="P22" s="15">
-        <f t="shared" ref="P22:P23" si="10">$C22*K22</f>
-        <v>0</v>
+        <f t="shared" ref="P22" si="15">$C22*K22</f>
+        <v>5</v>
       </c>
       <c r="Q22" s="15">
-        <f t="shared" ref="Q22:Q23" si="11">$C22*L22</f>
+        <f t="shared" ref="Q22" si="16">$C22*L22</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="6" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C23" s="10">
-        <v>2</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="4">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.5</v>
       </c>
       <c r="F23" s="4">
-        <v>0</v>
-      </c>
-      <c r="G23" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="4">
         <v>0</v>
       </c>
       <c r="H23" s="8">
@@ -1932,39 +1965,44 @@
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K23" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L23" s="4">
         <v>0</v>
       </c>
       <c r="M23" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="14"/>
       <c r="O23" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2.5</v>
       </c>
       <c r="P23" s="15">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2.5</v>
       </c>
       <c r="Q23" s="15">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="6" t="s">
-        <v>40</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>73</v>
       </c>
       <c r="C24" s="10">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -1981,7 +2019,7 @@
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="4">
         <v>0</v>
@@ -1991,12 +2029,12 @@
       </c>
       <c r="M24" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="14"/>
       <c r="O24" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P24" s="15">
         <f t="shared" si="4"/>
@@ -2007,22 +2045,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>41</v>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="44"/>
+      <c r="B25" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C25" s="10">
-        <v>2</v>
-      </c>
-      <c r="D25" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="E25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="4">
         <v>0</v>
@@ -2033,7 +2071,7 @@
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="4">
         <v>0</v>
@@ -2043,12 +2081,12 @@
       </c>
       <c r="M25" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="14"/>
       <c r="O25" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P25" s="15">
         <f t="shared" si="4"/>
@@ -2060,21 +2098,21 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="6" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C26" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0</v>
+        <v>71</v>
+      </c>
+      <c r="E26" s="46">
+        <v>0.25</v>
       </c>
       <c r="F26" s="4">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G26" s="4">
         <v>0</v>
@@ -2085,26 +2123,26 @@
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="3">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K26" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L26" s="4">
         <v>0</v>
       </c>
       <c r="M26" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="14"/>
       <c r="O26" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="P26" s="15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="Q26" s="15">
         <f t="shared" si="5"/>
@@ -2112,18 +2150,12 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
-      <c r="B27" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="10">
-        <v>1</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1</v>
+      <c r="A27" s="45"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="4">
+        <v>0</v>
       </c>
       <c r="F27" s="4">
         <v>0</v>
@@ -2133,7 +2165,7 @@
       </c>
       <c r="H27" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" s="13"/>
       <c r="J27" s="3">
@@ -2164,18 +2196,14 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="10">
-        <v>2</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="A28" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" s="4">
         <v>0</v>
@@ -2184,8 +2212,8 @@
         <v>0</v>
       </c>
       <c r="H28" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" ref="H28:H35" si="17">SUM(E28:G28)</f>
+        <v>0</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="3">
@@ -2203,22 +2231,20 @@
       </c>
       <c r="N28" s="14"/>
       <c r="O28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="O28:Q35" si="18">$C28*J28</f>
         <v>0</v>
       </c>
       <c r="P28" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q28" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
-        <v>45</v>
-      </c>
+      <c r="A29" s="44"/>
       <c r="B29" s="6"/>
       <c r="C29" s="10"/>
       <c r="D29" s="6"/>
@@ -2232,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="8">
-        <f t="shared" ref="H29:H36" si="12">SUM(E29:G29)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I29" s="13"/>
@@ -2251,20 +2277,20 @@
       </c>
       <c r="N29" s="14"/>
       <c r="O29" s="15">
-        <f>$C29*J29</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P29" s="15">
-        <f>$C29*K29</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q29" s="15">
-        <f>$C29*L29</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="6"/>
       <c r="C30" s="10"/>
       <c r="D30" s="6"/>
@@ -2278,7 +2304,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I30" s="13"/>
@@ -2297,20 +2323,20 @@
       </c>
       <c r="N30" s="14"/>
       <c r="O30" s="15">
-        <f>$C30*J30</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P30" s="15">
-        <f>$C30*K30</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q30" s="15">
-        <f>$C30*L30</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="6"/>
       <c r="C31" s="10"/>
       <c r="D31" s="6"/>
@@ -2324,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I31" s="13"/>
@@ -2343,20 +2369,20 @@
       </c>
       <c r="N31" s="14"/>
       <c r="O31" s="15">
-        <f>$C31*J31</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P31" s="15">
-        <f>$C31*K31</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q31" s="15">
-        <f>$C31*L31</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="6"/>
       <c r="C32" s="10"/>
       <c r="D32" s="6"/>
@@ -2370,7 +2396,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I32" s="13"/>
@@ -2389,20 +2415,20 @@
       </c>
       <c r="N32" s="14"/>
       <c r="O32" s="15">
-        <f>$C32*J32</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P32" s="15">
-        <f>$C32*K32</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q32" s="15">
-        <f>$C32*L32</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="6"/>
       <c r="C33" s="10"/>
       <c r="D33" s="6"/>
@@ -2416,7 +2442,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I33" s="13"/>
@@ -2435,20 +2461,20 @@
       </c>
       <c r="N33" s="14"/>
       <c r="O33" s="15">
-        <f>$C33*J33</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P33" s="15">
-        <f>$C33*K33</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q33" s="15">
-        <f>$C33*L33</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="6"/>
       <c r="C34" s="10"/>
       <c r="D34" s="6"/>
@@ -2462,7 +2488,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I34" s="13"/>
@@ -2481,20 +2507,20 @@
       </c>
       <c r="N34" s="14"/>
       <c r="O34" s="15">
-        <f>$C34*J34</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P34" s="15">
-        <f>$C34*K34</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q34" s="15">
-        <f>$C34*L34</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
+      <c r="A35" s="45"/>
       <c r="B35" s="6"/>
       <c r="C35" s="10"/>
       <c r="D35" s="6"/>
@@ -2508,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I35" s="13"/>
@@ -2527,110 +2553,77 @@
       </c>
       <c r="N35" s="14"/>
       <c r="O35" s="15">
-        <f>$C35*J35</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P35" s="15">
-        <f>$C35*K35</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q35" s="15">
-        <f>$C35*L35</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="4">
-        <v>0</v>
-      </c>
-      <c r="F36" s="4">
-        <v>0</v>
-      </c>
-      <c r="G36" s="4">
-        <v>0</v>
-      </c>
-      <c r="H36" s="8">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="I36" s="13"/>
-      <c r="J36" s="3">
-        <v>0</v>
-      </c>
-      <c r="K36" s="4">
-        <v>0</v>
-      </c>
-      <c r="L36" s="4">
-        <v>0</v>
-      </c>
-      <c r="M36" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N36" s="14"/>
-      <c r="O36" s="15">
-        <f>$C36*J36</f>
-        <v>0</v>
-      </c>
-      <c r="P36" s="15">
-        <f>$C36*K36</f>
-        <v>0</v>
-      </c>
-      <c r="Q36" s="15">
-        <f>$C36*L36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J37" s="34" t="s">
+      <c r="J36" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="O36" s="16">
+        <f>SUM(O10:O35)</f>
+        <v>36.75</v>
+      </c>
+      <c r="P36" s="16">
+        <f>SUM(P10:P35)</f>
+        <v>34.25</v>
+      </c>
+      <c r="Q36" s="16">
+        <f>SUM(Q10:Q35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="O37" s="16">
-        <f>SUM(O10:O36)</f>
-        <v>0</v>
-      </c>
-      <c r="P37" s="16">
-        <f>SUM(P10:P36)</f>
-        <v>0</v>
-      </c>
-      <c r="Q37" s="16">
-        <f>SUM(Q10:Q36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="31" t="s">
-        <v>21</v>
-      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="5" t="b">
+        <f>COUNTIF(D$10:D$35,"*"&amp;A40&amp;"*")&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B41" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A41&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A41&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
       <c r="D41" s="5"/>
@@ -2640,10 +2633,10 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B42" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A42&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A42&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
       <c r="D42" s="5"/>
@@ -2653,11 +2646,11 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B43" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A43&amp;"*")&gt;0</f>
-        <v>0</v>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A43&amp;"*")&gt;0</f>
+        <v>1</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="26"/>
@@ -2666,10 +2659,10 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B44" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A44&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A44&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
       <c r="D44" s="5"/>
@@ -2679,10 +2672,10 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B45" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A45&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A45&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
       <c r="D45" s="5"/>
@@ -2692,11 +2685,11 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B46" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A46&amp;"*")&gt;0</f>
-        <v>1</v>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A46&amp;"*")&gt;0</f>
+        <v>0</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="26"/>
@@ -2705,10 +2698,10 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B47" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A47&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A47&amp;"*")&gt;0</f>
         <v>0</v>
       </c>
       <c r="D47" s="5"/>
@@ -2718,10 +2711,10 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B48" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A48&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A48&amp;"*")&gt;0</f>
         <v>0</v>
       </c>
       <c r="D48" s="5"/>
@@ -2731,11 +2724,11 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B49" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A49&amp;"*")&gt;0</f>
-        <v>0</v>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A49&amp;"*")&gt;0</f>
+        <v>1</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="26"/>
@@ -2744,10 +2737,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B50" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A50&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A50&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
       <c r="D50" s="5"/>
@@ -2757,169 +2750,192 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="B51" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A51&amp;"*")&gt;0</f>
-        <v>1</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A51&amp;"*")&gt;0</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="28">
+        <f>SUM(E40:E50)</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="28">
+        <f t="shared" ref="F51:G51" si="19">SUM(F40:F50)</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="28">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B52" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A52&amp;"*")&gt;0</f>
-        <v>1</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E52" s="28">
-        <f>SUM(E41:E51)</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="28">
-        <f t="shared" ref="F52:G52" si="13">SUM(F41:F51)</f>
-        <v>0</v>
-      </c>
-      <c r="G52" s="28">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A52&amp;"*")&gt;0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B53" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A53&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A53&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B54" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A54&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A54&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B55" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A55&amp;"*")&gt;0</f>
-        <v>0</v>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A55&amp;"*")&gt;0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B56" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A56&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A56&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B57" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A57&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A57&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B58" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A58&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A58&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B59" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A59&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A59&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B60" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A60&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A60&amp;"*")&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B61" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A61&amp;"*")&gt;0</f>
-        <v>0</v>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A61&amp;"*")&gt;0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B62" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A62&amp;"*")&gt;0</f>
-        <v>0</v>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A62&amp;"*")&gt;0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B63" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A63&amp;"*")&gt;0</f>
-        <v>0</v>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A63&amp;"*")&gt;0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B64" s="5" t="b">
-        <f>COUNTIF(D$10:D$36,"*"&amp;A64&amp;"*")&gt;0</f>
+        <f>COUNTIF(D$10:D$35,"*"&amp;A64&amp;"*")&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="5" t="b">
+        <f>COUNTIF(D$10:D$35,"*"&amp;A65&amp;"*")&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="5" t="b">
+        <f>COUNTIF(D$10:D$35,"*"&amp;A66&amp;"*")&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" s="5" t="b">
+        <f>COUNTIF(D$10:D$35,"*"&amp;A67&amp;"*")&gt;0</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A23"/>
+    <mergeCell ref="J36:M36"/>
     <mergeCell ref="J7:Q7"/>
     <mergeCell ref="E7:H8"/>
     <mergeCell ref="J8:M8"/>
     <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A15:A24"/>
   </mergeCells>
-  <conditionalFormatting sqref="B41:B64">
+  <conditionalFormatting sqref="B40:B67">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:G36 J10:L36">
+  <conditionalFormatting sqref="E10:G35 J10:L35">
     <cfRule type="cellIs" dxfId="2" priority="8" operator="greaterThan">
       <formula>0.59</formula>
     </cfRule>

</xml_diff>